<commit_message>
RCM version added to AUS-22 CCLM5 simulations
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1.SAM-final" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3039" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3039" uniqueCount="215">
   <si>
     <t xml:space="preserve">1: South America (SAM): https://cordex.org/domains/cordex-region-south-america-cordex/ </t>
   </si>
@@ -576,9 +576,6 @@
   </si>
   <si>
     <t xml:space="preserve">ACCESS1-3_r1i1p1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCLM5-0-15</t>
   </si>
   <si>
     <t xml:space="preserve">CLMcom-HZG</t>
@@ -1909,7 +1906,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1975,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>78</v>
@@ -2013,13 +2010,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>48</v>
@@ -2034,7 +2031,7 @@
         <v>34</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>22</v>
@@ -2051,7 +2048,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -2089,13 +2086,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>48</v>
@@ -2127,7 +2124,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>50</v>
@@ -2165,13 +2162,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>48</v>
@@ -2203,7 +2200,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -2241,7 +2238,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -2279,7 +2276,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
@@ -2306,7 +2303,7 @@
         <v>22</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>32</v>
@@ -2317,7 +2314,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -2344,7 +2341,7 @@
         <v>22</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>32</v>
@@ -2355,7 +2352,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
@@ -2382,7 +2379,7 @@
         <v>22</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>32</v>
@@ -2414,8 +2411,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="1" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="12" style="1" width="10.67"/>
@@ -2425,7 +2422,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2491,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -2523,7 +2520,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -2555,7 +2552,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>35</v>
@@ -2587,7 +2584,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>118</v>
@@ -2608,16 +2605,16 @@
         <v>34</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="8" t="s">
+      <c r="L9" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2625,7 +2622,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>120</v>
@@ -2646,13 +2643,13 @@
         <v>34</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2660,7 +2657,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>38</v>
@@ -2681,16 +2678,16 @@
         <v>34</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="8" t="s">
+      <c r="L11" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="12" s="13" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2698,7 +2695,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>42</v>
@@ -2719,13 +2716,13 @@
         <v>20</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AMF12" s="15"/>
       <c r="AMG12" s="15"/>
@@ -2738,7 +2735,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
@@ -2765,7 +2762,7 @@
         <v>22</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>32</v>
@@ -2776,7 +2773,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>61</v>
@@ -2797,16 +2794,16 @@
         <v>19</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>212</v>
-      </c>
       <c r="L14" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2814,7 +2811,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>27</v>
@@ -2829,22 +2826,22 @@
         <v>19</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="8" t="s">
+      <c r="L15" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2852,7 +2849,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
@@ -2884,7 +2881,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>38</v>
@@ -2916,7 +2913,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>35</v>
@@ -2970,7 +2967,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="5" style="1" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1020" style="0" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.84"/>
@@ -10375,7 +10372,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -10858,8 +10855,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11331,7 +11328,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>44</v>
@@ -11346,7 +11343,7 @@
         <v>20</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>22</v>
@@ -11369,7 +11366,7 @@
         <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>85</v>
@@ -11384,7 +11381,7 @@
         <v>34</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>22</v>
@@ -11407,7 +11404,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>44</v>
@@ -11422,7 +11419,7 @@
         <v>34</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>22</v>
@@ -11445,7 +11442,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>44</v>
@@ -11483,7 +11480,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>44</v>
@@ -11521,7 +11518,7 @@
         <v>181</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>44</v>
@@ -11559,7 +11556,7 @@
         <v>181</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>44</v>
@@ -11597,7 +11594,7 @@
         <v>178</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>44</v>
@@ -11635,7 +11632,7 @@
         <v>178</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>44</v>
@@ -11667,28 +11664,28 @@
         <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>22</v>
@@ -11703,28 +11700,28 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>22</v>
@@ -11739,28 +11736,28 @@
         <v>22</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="F27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>22</v>
@@ -11775,28 +11772,28 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>22</v>
@@ -11811,28 +11808,28 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>22</v>
@@ -11847,28 +11844,28 @@
         <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="F30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>22</v>
@@ -11905,9 +11902,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="10.67"/>
@@ -11918,7 +11915,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11984,7 +11981,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>78</v>
@@ -12022,13 +12019,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>44</v>
@@ -12057,13 +12054,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>44</v>
@@ -12092,13 +12089,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>44</v>
@@ -12127,37 +12124,37 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>181</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="8" t="s">
+      <c r="L10" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12165,37 +12162,37 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="8" t="s">
+      <c r="L11" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12203,13 +12200,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>44</v>
@@ -12224,7 +12221,7 @@
         <v>34</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>22</v>
@@ -12239,13 +12236,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>44</v>
@@ -12260,7 +12257,7 @@
         <v>34</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>22</v>
@@ -12275,13 +12272,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>44</v>
@@ -12296,7 +12293,7 @@
         <v>34</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>22</v>
@@ -12311,13 +12308,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>44</v>
@@ -12332,7 +12329,7 @@
         <v>34</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>22</v>
@@ -12347,13 +12344,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>44</v>
@@ -12368,7 +12365,7 @@
         <v>34</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
CNRM-CM5 simulation eliminated for AUS-44i
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3039" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3029" uniqueCount="215">
   <si>
     <t xml:space="preserve">1: South America (SAM): https://cordex.org/domains/cordex-region-south-america-cordex/ </t>
   </si>
@@ -10853,10 +10853,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ30"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11667,7 +11667,7 @@
         <v>185</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>178</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>186</v>
@@ -11703,7 +11703,7 @@
         <v>185</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>186</v>
@@ -11739,7 +11739,7 @@
         <v>185</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>189</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>186</v>
@@ -11775,7 +11775,7 @@
         <v>185</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>186</v>
@@ -11811,7 +11811,7 @@
         <v>185</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>186</v>
@@ -11839,42 +11839,7 @@
       </c>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L30" s="3"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Error fixed in GCM_run name for AUS-44i-CanESM2 simulation
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3029" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3029" uniqueCount="214">
   <si>
     <t xml:space="preserve">1: South America (SAM): https://cordex.org/domains/cordex-region-south-america-cordex/ </t>
   </si>
@@ -597,9 +597,6 @@
   </si>
   <si>
     <t xml:space="preserve">CSIRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HadGEM2-CC_r1i1p1</t>
   </si>
   <si>
     <t xml:space="preserve">10: Antarctica (ANT): https://cordex.org/domains/region-10-antarctica/ </t>
@@ -1906,7 +1903,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1972,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>78</v>
@@ -2010,13 +2007,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>48</v>
@@ -2031,7 +2028,7 @@
         <v>34</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>22</v>
@@ -2048,7 +2045,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -2086,13 +2083,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>48</v>
@@ -2124,7 +2121,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>50</v>
@@ -2162,13 +2159,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>48</v>
@@ -2200,7 +2197,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -2238,7 +2235,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -2276,7 +2273,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
@@ -2303,7 +2300,7 @@
         <v>22</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>32</v>
@@ -2314,7 +2311,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -2341,7 +2338,7 @@
         <v>22</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>32</v>
@@ -2352,7 +2349,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
@@ -2379,7 +2376,7 @@
         <v>22</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>32</v>
@@ -2422,7 +2419,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2488,7 +2485,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -2520,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -2552,7 +2549,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>35</v>
@@ -2584,7 +2581,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>118</v>
@@ -2605,16 +2602,16 @@
         <v>34</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="8" t="s">
+      <c r="L9" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2622,7 +2619,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>120</v>
@@ -2643,13 +2640,13 @@
         <v>34</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2657,7 +2654,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>38</v>
@@ -2678,16 +2675,16 @@
         <v>34</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="8" t="s">
+      <c r="L11" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="12" s="13" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2695,7 +2692,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>42</v>
@@ -2716,13 +2713,13 @@
         <v>20</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AMF12" s="15"/>
       <c r="AMG12" s="15"/>
@@ -2735,7 +2732,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
@@ -2762,7 +2759,7 @@
         <v>22</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>32</v>
@@ -2773,7 +2770,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>61</v>
@@ -2794,16 +2791,16 @@
         <v>19</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>211</v>
-      </c>
       <c r="L14" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2811,7 +2808,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>27</v>
@@ -2826,22 +2823,22 @@
         <v>19</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="8" t="s">
+      <c r="L15" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2849,7 +2846,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
@@ -2881,7 +2878,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>38</v>
@@ -2913,7 +2910,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>35</v>
@@ -10856,7 +10853,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11703,7 +11700,7 @@
         <v>185</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>189</v>
+        <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>186</v>
@@ -11880,7 +11877,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11946,7 +11943,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>78</v>
@@ -11984,13 +11981,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>44</v>
@@ -12019,13 +12016,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>44</v>
@@ -12054,13 +12051,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>44</v>
@@ -12089,37 +12086,37 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>181</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="8" t="s">
+      <c r="L10" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12127,37 +12124,37 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="8" t="s">
+      <c r="L11" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12165,7 +12162,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>178</v>
@@ -12201,7 +12198,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>16</v>
@@ -12237,7 +12234,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>42</v>
@@ -12273,7 +12270,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
@@ -12309,7 +12306,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Discarded simulations for AFR domain due to problems with precipitation units (RegCM4-3_v4)
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1.SAM-final" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="212">
   <si>
     <t xml:space="preserve">1: South America (SAM): https://cordex.org/domains/cordex-region-south-america-cordex/ </t>
   </si>
@@ -483,6 +483,9 @@
   </si>
   <si>
     <t xml:space="preserve">DOI:10.1002/2017EF000714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discarded due to problems with units in precipitation</t>
   </si>
   <si>
     <t xml:space="preserve">RACMO22T_v1</t>
@@ -672,7 +675,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -722,6 +725,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFED1C24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -778,7 +794,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -859,6 +875,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -922,7 +950,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -1894,7 +1922,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1960,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>78</v>
@@ -1998,13 +2026,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>48</v>
@@ -2019,7 +2047,7 @@
         <v>34</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>22</v>
@@ -2036,7 +2064,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -2074,13 +2102,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>48</v>
@@ -2112,7 +2140,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>50</v>
@@ -2150,13 +2178,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>48</v>
@@ -2188,7 +2216,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -2226,7 +2254,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -2264,7 +2292,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
@@ -2291,7 +2319,7 @@
         <v>22</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>32</v>
@@ -2302,7 +2330,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -2329,7 +2357,7 @@
         <v>22</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>32</v>
@@ -2340,7 +2368,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
@@ -2367,7 +2395,7 @@
         <v>22</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>32</v>
@@ -2399,8 +2427,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="1" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="12" style="1" width="10.67"/>
@@ -2410,7 +2438,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2476,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -2508,7 +2536,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -2540,7 +2568,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>35</v>
@@ -2572,7 +2600,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>115</v>
@@ -2593,16 +2621,16 @@
         <v>34</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2610,7 +2638,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>117</v>
@@ -2631,13 +2659,13 @@
         <v>34</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2645,7 +2673,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>38</v>
@@ -2666,16 +2694,16 @@
         <v>34</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" s="13" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2683,7 +2711,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>42</v>
@@ -2704,13 +2732,13 @@
         <v>20</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AMF12" s="15"/>
       <c r="AMG12" s="15"/>
@@ -2723,7 +2751,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
@@ -2750,7 +2778,7 @@
         <v>22</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>32</v>
@@ -2761,7 +2789,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>61</v>
@@ -2782,16 +2810,16 @@
         <v>19</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2799,7 +2827,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>27</v>
@@ -2814,22 +2842,22 @@
         <v>19</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2837,7 +2865,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
@@ -2869,7 +2897,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>38</v>
@@ -2901,7 +2929,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>35</v>
@@ -2955,7 +2983,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="5" style="1" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1020" style="0" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.84"/>
@@ -4687,7 +4715,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -7582,8 +7610,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8366,79 +8394,79 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="6" t="s">
+      <c r="F24" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="1" t="s">
+      <c r="J24" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="20" t="s">
         <v>23</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>32</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="A25" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="6" t="s">
+      <c r="F25" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>32</v>
+      <c r="J25" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8452,7 +8480,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>44</v>
@@ -8490,7 +8518,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>44</v>
@@ -9060,7 +9088,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>16</v>
@@ -9131,7 +9159,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9200,7 +9228,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>50</v>
@@ -9235,7 +9263,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -9270,7 +9298,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>35</v>
@@ -9282,7 +9310,7 @@
         <v>44</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>19</v>
@@ -9297,7 +9325,7 @@
         <v>22</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9305,7 +9333,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -9343,7 +9371,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -9381,7 +9409,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
@@ -9419,7 +9447,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
@@ -9440,7 +9468,7 @@
         <v>20</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>22</v>
@@ -9449,7 +9477,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9457,7 +9485,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>38</v>
@@ -9478,7 +9506,7 @@
         <v>20</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>22</v>
@@ -9487,7 +9515,7 @@
         <v>23</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9495,7 +9523,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>35</v>
@@ -9516,7 +9544,7 @@
         <v>20</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>22</v>
@@ -9525,7 +9553,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9533,13 +9561,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>48</v>
@@ -9554,7 +9582,7 @@
         <v>20</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>22</v>
@@ -9571,13 +9599,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>48</v>
@@ -9589,10 +9617,10 @@
         <v>20</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>22</v>
@@ -9609,13 +9637,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>48</v>
@@ -9630,7 +9658,7 @@
         <v>20</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>22</v>
@@ -9647,13 +9675,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>117</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>48</v>
@@ -9668,7 +9696,7 @@
         <v>20</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>22</v>
@@ -9685,13 +9713,13 @@
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>48</v>
@@ -9706,7 +9734,7 @@
         <v>20</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>22</v>
@@ -9723,13 +9751,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>48</v>
@@ -9744,7 +9772,7 @@
         <v>20</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>22</v>
@@ -9761,7 +9789,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>33</v>
@@ -9788,7 +9816,7 @@
         <v>22</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>32</v>
@@ -9799,13 +9827,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>48</v>
@@ -9837,13 +9865,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>48</v>
@@ -9875,13 +9903,13 @@
         <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>48</v>
@@ -9913,13 +9941,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>48</v>
@@ -9951,13 +9979,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>48</v>
@@ -9989,13 +10017,13 @@
         <v>22</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>48</v>
@@ -10027,13 +10055,13 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>48</v>
@@ -10065,13 +10093,13 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>48</v>
@@ -10103,13 +10131,13 @@
         <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>48</v>
@@ -10141,13 +10169,13 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>48</v>
@@ -10208,7 +10236,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10277,7 +10305,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -10312,7 +10340,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -10347,7 +10375,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>35</v>
@@ -10382,13 +10410,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>48</v>
@@ -10417,13 +10445,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>48</v>
@@ -10452,13 +10480,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>48</v>
@@ -10487,13 +10515,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>48</v>
@@ -10522,7 +10550,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>78</v>
@@ -10557,13 +10585,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>30</v>
@@ -10592,16 +10620,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>20</v>
@@ -10627,13 +10655,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>30</v>
@@ -10693,7 +10721,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10762,7 +10790,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -10800,7 +10828,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -10838,7 +10866,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>35</v>
@@ -10876,7 +10904,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -10914,7 +10942,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>38</v>
@@ -10952,7 +10980,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
@@ -10990,13 +11018,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>48</v>
@@ -11028,13 +11056,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>48</v>
@@ -11066,13 +11094,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>48</v>
@@ -11087,7 +11115,7 @@
         <v>19</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>22</v>
@@ -11104,13 +11132,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>48</v>
@@ -11125,7 +11153,7 @@
         <v>19</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>22</v>
@@ -11142,7 +11170,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
@@ -11163,7 +11191,7 @@
         <v>20</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>22</v>
@@ -11180,7 +11208,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>33</v>
@@ -11201,7 +11229,7 @@
         <v>34</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>22</v>
@@ -11218,7 +11246,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>35</v>
@@ -11239,7 +11267,7 @@
         <v>34</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>22</v>
@@ -11256,13 +11284,13 @@
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>44</v>
@@ -11277,7 +11305,7 @@
         <v>34</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>22</v>
@@ -11294,13 +11322,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>44</v>
@@ -11315,7 +11343,7 @@
         <v>34</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>22</v>
@@ -11332,13 +11360,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>44</v>
@@ -11353,7 +11381,7 @@
         <v>34</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>22</v>
@@ -11370,13 +11398,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>44</v>
@@ -11391,7 +11419,7 @@
         <v>34</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>22</v>
@@ -11408,13 +11436,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>44</v>
@@ -11429,7 +11457,7 @@
         <v>34</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>22</v>
@@ -11446,13 +11474,13 @@
         <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>44</v>
@@ -11467,7 +11495,7 @@
         <v>34</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>22</v>
@@ -11484,16 +11512,16 @@
         <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>19</v>
@@ -11505,7 +11533,7 @@
         <v>20</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>22</v>
@@ -11520,16 +11548,16 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>19</v>
@@ -11541,7 +11569,7 @@
         <v>20</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>22</v>
@@ -11556,16 +11584,16 @@
         <v>22</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>19</v>
@@ -11577,7 +11605,7 @@
         <v>20</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>22</v>
@@ -11592,16 +11620,16 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>19</v>
@@ -11613,7 +11641,7 @@
         <v>20</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>22</v>
@@ -11628,16 +11656,16 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>19</v>
@@ -11649,7 +11677,7 @@
         <v>20</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>22</v>
@@ -11686,9 +11714,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="10.67"/>
@@ -11699,7 +11727,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11765,7 +11793,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>78</v>
@@ -11803,13 +11831,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>44</v>
@@ -11838,13 +11866,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>44</v>
@@ -11873,13 +11901,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>44</v>
@@ -11908,16 +11936,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>19</v>
@@ -11929,16 +11957,16 @@
         <v>34</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11946,16 +11974,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
@@ -11967,16 +11995,16 @@
         <v>34</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11984,13 +12012,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>44</v>
@@ -12005,7 +12033,7 @@
         <v>34</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>22</v>
@@ -12020,13 +12048,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>44</v>
@@ -12041,7 +12069,7 @@
         <v>34</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>22</v>
@@ -12056,13 +12084,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>44</v>
@@ -12077,7 +12105,7 @@
         <v>34</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>22</v>
@@ -12092,13 +12120,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>44</v>
@@ -12113,7 +12141,7 @@
         <v>34</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>22</v>
@@ -12128,13 +12156,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>44</v>
@@ -12149,7 +12177,7 @@
         <v>34</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
rcp85 scenario is only available for EUR-11_WRF361H_v1
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1.SAM-final" sheetId="1" state="visible" r:id="rId2"/>
@@ -675,7 +675,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -733,12 +733,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -794,7 +788,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -880,10 +874,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4715,8 +4705,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6483,11 +6473,11 @@
       <c r="D45" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E45" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>34</v>
+      <c r="E45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>19</v>
@@ -7610,7 +7600,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -8465,7 +8455,7 @@
       <c r="K25" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="L25" s="22" t="s">
+      <c r="L25" s="8" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Index numbers updated for all the domains
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="1.SAM-final" sheetId="1" state="visible" r:id="rId2"/>
@@ -957,7 +957,7 @@
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1893,7 +1893,7 @@
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2409,8 +2409,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2697,7 +2697,7 @@
       </c>
     </row>
     <row r="12" s="13" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -2965,7 +2965,7 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3349,7 +3349,7 @@
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>58</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>58</v>
@@ -3425,7 +3425,7 @@
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>58</v>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>58</v>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>58</v>
@@ -3539,7 +3539,7 @@
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>58</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>58</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>58</v>
@@ -3653,7 +3653,7 @@
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>58</v>
@@ -3691,7 +3691,7 @@
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>58</v>
@@ -3729,7 +3729,7 @@
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>58</v>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>55</v>
@@ -3805,7 +3805,7 @@
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>72</v>
@@ -3857,7 +3857,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4313,7 +4313,7 @@
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>81</v>
@@ -4351,7 +4351,7 @@
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>81</v>
@@ -4389,7 +4389,7 @@
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>81</v>
@@ -4427,7 +4427,7 @@
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>81</v>
@@ -4465,7 +4465,7 @@
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>81</v>
@@ -4503,7 +4503,7 @@
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>81</v>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>81</v>
@@ -4579,7 +4579,7 @@
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>81</v>
@@ -4615,9 +4615,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>81</v>
@@ -4651,9 +4651,9 @@
       </c>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>81</v>
@@ -4705,8 +4705,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7601,7 +7601,7 @@
   <dimension ref="A1:AMJ42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7910,7 +7910,7 @@
       </c>
     </row>
     <row r="12" s="13" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -7954,7 +7954,7 @@
       <c r="AMJ12" s="15"/>
     </row>
     <row r="13" s="13" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -7998,7 +7998,7 @@
       <c r="AMJ13" s="15"/>
     </row>
     <row r="14" s="13" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -8384,7 +8384,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="n">
+      <c r="A24" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B24" s="20" t="s">
@@ -8422,7 +8422,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="n">
+      <c r="A25" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B25" s="20" t="s">
@@ -8499,7 +8499,7 @@
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>149</v>
@@ -8537,7 +8537,7 @@
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>149</v>
@@ -8575,7 +8575,7 @@
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>149</v>
@@ -8613,7 +8613,7 @@
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>149</v>
@@ -8651,7 +8651,7 @@
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>149</v>
@@ -8689,7 +8689,7 @@
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>149</v>
@@ -8727,7 +8727,7 @@
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>149</v>
@@ -8765,7 +8765,7 @@
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>149</v>
@@ -8803,7 +8803,7 @@
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>149</v>
@@ -8841,7 +8841,7 @@
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>149</v>
@@ -8879,7 +8879,7 @@
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>149</v>
@@ -8917,7 +8917,7 @@
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>149</v>
@@ -8955,7 +8955,7 @@
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>149</v>
@@ -8992,8 +8992,8 @@
       </c>
     </row>
     <row r="40" s="13" customFormat="true" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="n">
-        <v>40</v>
+      <c r="A40" s="1" t="n">
+        <v>35</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>149</v>
@@ -9037,7 +9037,7 @@
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>149</v>
@@ -9075,7 +9075,7 @@
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>154</v>
@@ -9130,7 +9130,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10211,7 +10211,7 @@
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10694,7 +10694,7 @@
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11497,7 +11497,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>20</v>
       </c>
@@ -11533,7 +11533,7 @@
       </c>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>21</v>
       </c>
@@ -11569,7 +11569,7 @@
       </c>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>22</v>
       </c>
@@ -11605,7 +11605,7 @@
       </c>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>23</v>
       </c>
@@ -11641,7 +11641,7 @@
       </c>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>24</v>
       </c>
@@ -11696,7 +11696,7 @@
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Eliminated r12i1p1 run for RACMO21P_v1 for ANT domain
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CORDEX_simulations_ATLAS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="1.SAM-final" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="212">
   <si>
     <t xml:space="preserve">1: South America (SAM): https://cordex.org/domains/cordex-region-south-america-cordex/ </t>
   </si>
@@ -2409,7 +2409,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -11693,10 +11693,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ16"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11824,7 +11824,7 @@
         <v>189</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>190</v>
@@ -11832,14 +11832,14 @@
       <c r="E7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>19</v>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>131</v>
@@ -11859,16 +11859,16 @@
         <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>19</v>
+      <c r="F8" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>34</v>
@@ -11894,31 +11894,34 @@
         <v>189</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>34</v>
+        <v>172</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>131</v>
+        <v>193</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>23</v>
+        <v>194</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11929,7 +11932,7 @@
         <v>189</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>180</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>192</v>
@@ -11964,38 +11967,36 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>177</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>172</v>
+        <v>44</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
+      <c r="G11" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>195</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -12005,7 +12006,7 @@
         <v>196</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>177</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>185</v>
@@ -12041,7 +12042,7 @@
         <v>196</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>185</v>
@@ -12077,7 +12078,7 @@
         <v>196</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>185</v>
@@ -12113,7 +12114,7 @@
         <v>196</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>185</v>
@@ -12141,42 +12142,7 @@
       </c>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="3"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>